<commit_message>
Readmes added to templates
</commit_message>
<xml_diff>
--- a/gbif-ipt-docs/downloads/checklist_ipt_template_v1.xlsx
+++ b/gbif-ipt-docs/downloads/checklist_ipt_template_v1.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="21740" yWindow="0" windowWidth="16640" windowHeight="7420" tabRatio="500"/>
+    <workbookView xWindow="17800" yWindow="4060" windowWidth="17340" windowHeight="13280" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Classification" sheetId="1" r:id="rId1"/>
+    <sheet name="README" sheetId="2" r:id="rId1"/>
+    <sheet name="Classification" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -279,7 +280,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>taxonID</t>
   </si>
@@ -297,13 +298,99 @@
   </si>
   <si>
     <t>acceptedNameUsageID</t>
+  </si>
+  <si>
+    <t>GBIF IPT Template:</t>
+  </si>
+  <si>
+    <t>Checklist Data</t>
+  </si>
+  <si>
+    <t>Use this template for filling in a species list or taxonomy. Upload the template to the IPT where it can be published in Darwin Core Archive (DwC-A) format. Note this template must be mapped to the Taxon Core in the IPT.</t>
+  </si>
+  <si>
+    <t>Sheet Name</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Classification</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This sheet is used to record the species list. For filling in a taxonomy, make sure the classification uses a parent ID (parentNameUsageID) related to the primary taxonID as the means of recording the taxonomic hierarchy.</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>#1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The header row shows required and recommended terms. Hover over the cell to find out if it's required or recommended, and to obtain a definition of the term examples. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>#2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Additional columns can be added, but you should use DwC term names: http://rs.tdwg.org/dwc/terms/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>#3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Columns can be reordered, but the header name (equal to a DwC term name) cannot be changed.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -365,8 +452,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="23"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,8 +501,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="43"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -406,6 +529,92 @@
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="23"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -429,11 +638,50 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -781,10 +1029,108 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="85.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="20">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="6"/>
+      <c r="B3" s="8"/>
+    </row>
+    <row r="4" spans="1:2" ht="45">
+      <c r="A4" s="6"/>
+      <c r="B4" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="10"/>
+    </row>
+    <row r="6" spans="1:2" ht="16" thickBot="1">
+      <c r="A6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="45">
+      <c r="A7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="14"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="16"/>
+      <c r="B9" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30">
+      <c r="A10" s="18"/>
+      <c r="B10" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30">
+      <c r="A11" s="18"/>
+      <c r="B11" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="18"/>
+      <c r="B12" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adds checklist template with data
</commit_message>
<xml_diff>
--- a/gbif-ipt-docs/downloads/checklist_ipt_template_v1.xlsx
+++ b/gbif-ipt-docs/downloads/checklist_ipt_template_v1.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17800" yWindow="4060" windowWidth="17340" windowHeight="13280" tabRatio="500"/>
+    <workbookView xWindow="2780" yWindow="5880" windowWidth="23200" windowHeight="7200" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="README" sheetId="2" r:id="rId1"/>
-    <sheet name="Classification" sheetId="1" r:id="rId2"/>
+    <sheet name="Classification" sheetId="1" r:id="rId1"/>
+    <sheet name="README" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -154,7 +154,7 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>RECOMMENDED
+          <t>REQUIRED
 Definition:</t>
         </r>
         <r>
@@ -163,25 +163,35 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve"> The full scientific name of the kingdom in which the taxon is classified.
+          <t xml:space="preserve"> The full scientific name, with authorship and date information if known. When forming part of an Identification, this should be the name in lowest level taxonomic rank that can be determined. This term should not contain identification qualifications, which should instead be supplied in the identificationQualifier term.
 </t>
         </r>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
             <b/>
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">Examples: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve"> "Animalia", "Plantae".</t>
+          <t>Examples:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> "Roptrocerus typographi (Györfi, 1952)" (genus + specificEpithet + scientificNameAuthorship), "Quercus agrifolia var. oxyadenia (Torr.) J.T. Howell" (genus + specificEpithet + taxonRank + infraspecificEpithet + scientificNameAuthorship), "Coleoptera" (order), "Vespertilionidae" (family), "Manis" (genus), "Ctenomys sociabilis" (genus + specificEpithet), "Ambystoma tigrinum diaboli" (genus + specificEpithet + infraspecificEpithet).</t>
         </r>
       </text>
     </comment>
@@ -194,7 +204,7 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>REQUIRED
+          <t>RECOMMENDED
 Definition:</t>
         </r>
         <r>
@@ -203,35 +213,25 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve"> The full scientific name, with authorship and date information if known. When forming part of an Identification, this should be the name in lowest level taxonomic rank that can be determined. This term should not contain identification qualifications, which should instead be supplied in the identificationQualifier term.
+          <t xml:space="preserve"> The full scientific name of the kingdom in which the taxon is classified.
 </t>
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
             <b/>
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>Examples:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve"> "Roptrocerus typographi (Györfi, 1952)" (genus + specificEpithet + scientificNameAuthorship), "Quercus agrifolia var. oxyadenia (Torr.) J.T. Howell" (genus + specificEpithet + taxonRank + infraspecificEpithet + scientificNameAuthorship), "Coleoptera" (order), "Vespertilionidae" (family), "Manis" (genus), "Ctenomys sociabilis" (genus + specificEpithet), "Ambystoma tigrinum diaboli" (genus + specificEpithet + infraspecificEpithet).</t>
+          <t xml:space="preserve">Examples: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> "Animalia", "Plantae".</t>
         </r>
       </text>
     </comment>
@@ -618,9 +618,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="18">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -683,7 +685,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -692,6 +694,7 @@
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -700,6 +703,7 @@
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
@@ -1029,10 +1033,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="6" width="11.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="B2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1124,56 +1179,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="B2" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
More updates to templates
</commit_message>
<xml_diff>
--- a/gbif-ipt-docs/downloads/checklist_ipt_template_v1.xlsx
+++ b/gbif-ipt-docs/downloads/checklist_ipt_template_v1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="5880" windowWidth="23200" windowHeight="7200" tabRatio="500"/>
+    <workbookView xWindow="2460" yWindow="900" windowWidth="22420" windowHeight="14360" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Classification" sheetId="1" r:id="rId1"/>
@@ -1036,7 +1036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1087,9 +1087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>

</xml_diff>

<commit_message>
More changes to templates
</commit_message>
<xml_diff>
--- a/gbif-ipt-docs/downloads/checklist_ipt_template_v1.xlsx
+++ b/gbif-ipt-docs/downloads/checklist_ipt_template_v1.xlsx
@@ -280,7 +280,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>taxonID</t>
   </si>
@@ -383,6 +383,32 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> Columns can be reordered, but the header name (equal to a DwC term name) cannot be changed.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>#</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Enter lists using the pipe (“|”) character as a separator, for applicable DwC terms only.</t>
     </r>
   </si>
 </sst>
@@ -618,7 +644,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -639,8 +665,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -684,8 +712,11 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="20">
+  <cellStyles count="22">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -695,6 +726,7 @@
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -704,6 +736,7 @@
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
@@ -1165,12 +1198,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="18" customHeight="1">
       <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
+      <c r="B13" s="21" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>